<commit_message>
MAJ dico de données
</commit_message>
<xml_diff>
--- a/bdd/dico_de_donnees.xlsx
+++ b/bdd/dico_de_donnees.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="70">
   <si>
     <t xml:space="preserve">DICTIONNAIRE DE DONNEES</t>
   </si>
@@ -97,21 +97,6 @@
     <t xml:space="preserve">mot de passe d'accès Pandora</t>
   </si>
   <si>
-    <t xml:space="preserve">PROFIL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IdProf</t>
-  </si>
-  <si>
-    <t xml:space="preserve">identifiant profil utilisateur</t>
-  </si>
-  <si>
-    <t xml:space="preserve">typeProf</t>
-  </si>
-  <si>
-    <t xml:space="preserve">type de profile utilisateur</t>
-  </si>
-  <si>
     <t xml:space="preserve">ANNONCES</t>
   </si>
   <si>
@@ -203,21 +188,6 @@
   </si>
   <si>
     <t xml:space="preserve">date de publication commentaire</t>
-  </si>
-  <si>
-    <t xml:space="preserve">THEME FURUM</t>
-  </si>
-  <si>
-    <t xml:space="preserve">idTheme</t>
-  </si>
-  <si>
-    <t xml:space="preserve">identifiant du theme</t>
-  </si>
-  <si>
-    <t xml:space="preserve">typeTh</t>
-  </si>
-  <si>
-    <t xml:space="preserve">type du theme</t>
   </si>
   <si>
     <t xml:space="preserve">SUJET THEME</t>
@@ -346,7 +316,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="19">
+  <borders count="18">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
@@ -482,7 +452,7 @@
       <left style="thin">
         <color rgb="FF666666"/>
       </left>
-      <right style="thin">
+      <right style="thick">
         <color rgb="FF666666"/>
       </right>
       <top style="thin">
@@ -497,7 +467,7 @@
       <left style="thin">
         <color rgb="FF666666"/>
       </left>
-      <right style="thick">
+      <right style="thin">
         <color rgb="FF666666"/>
       </right>
       <top style="thin">
@@ -539,17 +509,6 @@
       <bottom style="thin">
         <color rgb="FF666666"/>
       </bottom>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="thin">
-        <color rgb="FF666666"/>
-      </left>
-      <right style="thick"/>
-      <top style="thin">
-        <color rgb="FF666666"/>
-      </top>
-      <bottom/>
       <diagonal/>
     </border>
     <border diagonalUp="false" diagonalDown="false">
@@ -604,7 +563,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="20">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -653,11 +612,11 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="4" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="6" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="6" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="4" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -673,11 +632,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="6" borderId="16" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="4" borderId="17" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="4" borderId="16" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -685,7 +640,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="6" borderId="18" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="6" borderId="17" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -766,16 +721,16 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="true"/>
   </sheetPr>
-  <dimension ref="A1:I36"/>
+  <dimension ref="A1:I1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A26" activeCellId="0" sqref="A26"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.4453125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.4609375" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="28.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="28.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="28.98"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -960,7 +915,7 @@
       </c>
       <c r="I10" s="7"/>
     </row>
-    <row r="11" customFormat="false" ht="30.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="31.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="9" t="s">
         <v>25</v>
       </c>
@@ -981,55 +936,53 @@
         <v>11</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="31.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="33.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="9"/>
       <c r="B12" s="9"/>
-      <c r="C12" s="12" t="s">
+      <c r="C12" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="D12" s="12"/>
-      <c r="E12" s="12" t="s">
+      <c r="D12" s="6"/>
+      <c r="E12" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="F12" s="12"/>
-      <c r="G12" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="H12" s="12" t="n">
-        <v>255</v>
-      </c>
-      <c r="I12" s="13"/>
-    </row>
-    <row r="13" customFormat="false" ht="31.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A13" s="9" t="s">
+      <c r="F12" s="6"/>
+      <c r="G12" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="H12" s="6" t="n">
+        <v>255</v>
+      </c>
+      <c r="I12" s="12"/>
+    </row>
+    <row r="13" customFormat="false" ht="34.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A13" s="9"/>
+      <c r="B13" s="9"/>
+      <c r="C13" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="B13" s="9"/>
-      <c r="C13" s="10" t="s">
+      <c r="D13" s="6"/>
+      <c r="E13" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="D13" s="10"/>
-      <c r="E13" s="10" t="s">
-        <v>32</v>
-      </c>
-      <c r="F13" s="10"/>
-      <c r="G13" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="H13" s="10"/>
-      <c r="I13" s="11" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="33.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="F13" s="6"/>
+      <c r="G13" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="H13" s="6" t="n">
+        <v>255</v>
+      </c>
+      <c r="I13" s="12"/>
+    </row>
+    <row r="14" customFormat="false" ht="31.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="9"/>
       <c r="B14" s="9"/>
       <c r="C14" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D14" s="6"/>
       <c r="E14" s="6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F14" s="6"/>
       <c r="G14" s="6" t="s">
@@ -1038,17 +991,17 @@
       <c r="H14" s="6" t="n">
         <v>255</v>
       </c>
-      <c r="I14" s="13"/>
-    </row>
-    <row r="15" customFormat="false" ht="34.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="I14" s="12"/>
+    </row>
+    <row r="15" customFormat="false" ht="33" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="9"/>
       <c r="B15" s="9"/>
       <c r="C15" s="6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D15" s="6"/>
       <c r="E15" s="6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F15" s="6"/>
       <c r="G15" s="6" t="s">
@@ -1057,26 +1010,24 @@
       <c r="H15" s="6" t="n">
         <v>255</v>
       </c>
-      <c r="I15" s="13"/>
+      <c r="I15" s="12"/>
     </row>
     <row r="16" customFormat="false" ht="31.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="9"/>
       <c r="B16" s="9"/>
       <c r="C16" s="6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D16" s="6"/>
       <c r="E16" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F16" s="6"/>
       <c r="G16" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="H16" s="6" t="n">
-        <v>255</v>
-      </c>
-      <c r="I16" s="13"/>
+        <v>38</v>
+      </c>
+      <c r="H16" s="6"/>
+      <c r="I16" s="12"/>
     </row>
     <row r="17" customFormat="false" ht="33" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="9"/>
@@ -1095,72 +1046,74 @@
       <c r="H17" s="6" t="n">
         <v>255</v>
       </c>
-      <c r="I17" s="13"/>
-    </row>
-    <row r="18" customFormat="false" ht="31.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="I17" s="12"/>
+    </row>
+    <row r="18" customFormat="false" ht="32.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="9"/>
       <c r="B18" s="9"/>
-      <c r="C18" s="6" t="s">
+      <c r="C18" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="D18" s="6"/>
-      <c r="E18" s="6" t="s">
+      <c r="D18" s="8"/>
+      <c r="E18" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="F18" s="6"/>
-      <c r="G18" s="6" t="s">
+      <c r="F18" s="8"/>
+      <c r="G18" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="H18" s="8"/>
+      <c r="I18" s="12"/>
+    </row>
+    <row r="19" customFormat="false" ht="31.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A19" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="H18" s="6"/>
-      <c r="I18" s="13"/>
-    </row>
-    <row r="19" customFormat="false" ht="33" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A19" s="9"/>
       <c r="B19" s="9"/>
-      <c r="C19" s="6" t="s">
+      <c r="C19" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="D19" s="6"/>
-      <c r="E19" s="6" t="s">
+      <c r="D19" s="10"/>
+      <c r="E19" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="F19" s="6"/>
-      <c r="G19" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="H19" s="6" t="n">
-        <v>255</v>
-      </c>
-      <c r="I19" s="13"/>
+      <c r="F19" s="10"/>
+      <c r="G19" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="H19" s="10"/>
+      <c r="I19" s="11" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="20" customFormat="false" ht="32.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="9"/>
       <c r="B20" s="9"/>
-      <c r="C20" s="8" t="s">
+      <c r="C20" s="13" t="s">
         <v>46</v>
       </c>
-      <c r="D20" s="8"/>
-      <c r="E20" s="8" t="s">
+      <c r="D20" s="13"/>
+      <c r="E20" s="13" t="s">
         <v>47</v>
       </c>
-      <c r="F20" s="8"/>
-      <c r="G20" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="H20" s="8"/>
-      <c r="I20" s="13"/>
-    </row>
-    <row r="21" customFormat="false" ht="31.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="F20" s="13"/>
+      <c r="G20" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="H20" s="13"/>
+      <c r="I20" s="12"/>
+    </row>
+    <row r="21" customFormat="false" ht="33" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="9" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B21" s="9"/>
       <c r="C21" s="10" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D21" s="10"/>
       <c r="E21" s="10" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="F21" s="10"/>
       <c r="G21" s="10" t="s">
@@ -1171,81 +1124,83 @@
         <v>11</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="32.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="22" customFormat="false" ht="33" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="9"/>
       <c r="B22" s="9"/>
-      <c r="C22" s="12" t="s">
-        <v>51</v>
-      </c>
-      <c r="D22" s="12"/>
-      <c r="E22" s="12" t="s">
+      <c r="C22" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="F22" s="12"/>
-      <c r="G22" s="12" t="s">
+      <c r="D22" s="6"/>
+      <c r="E22" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="H22" s="12"/>
-      <c r="I22" s="13"/>
-    </row>
-    <row r="23" customFormat="false" ht="33" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A23" s="9" t="s">
+      <c r="F22" s="6"/>
+      <c r="G22" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="H22" s="6" t="n">
+        <v>255</v>
+      </c>
+      <c r="I22" s="12"/>
+    </row>
+    <row r="23" customFormat="false" ht="47.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A23" s="9"/>
+      <c r="B23" s="9"/>
+      <c r="C23" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="B23" s="9"/>
-      <c r="C23" s="10" t="s">
+      <c r="D23" s="8"/>
+      <c r="E23" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="D23" s="10"/>
-      <c r="E23" s="10" t="s">
+      <c r="F23" s="8"/>
+      <c r="G23" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="H23" s="8"/>
+      <c r="I23" s="12"/>
+    </row>
+    <row r="24" customFormat="false" ht="40.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A24" s="14" t="s">
         <v>56</v>
       </c>
-      <c r="F23" s="10"/>
-      <c r="G23" s="10" t="s">
+      <c r="B24" s="14"/>
+      <c r="C24" s="15" t="s">
+        <v>57</v>
+      </c>
+      <c r="D24" s="15"/>
+      <c r="E24" s="15" t="s">
+        <v>58</v>
+      </c>
+      <c r="F24" s="15"/>
+      <c r="G24" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="H23" s="10"/>
-      <c r="I23" s="11" t="s">
+      <c r="H24" s="15"/>
+      <c r="I24" s="16" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="33" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A24" s="9"/>
-      <c r="B24" s="9"/>
-      <c r="C24" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="D24" s="6"/>
-      <c r="E24" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="F24" s="6"/>
-      <c r="G24" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="H24" s="6" t="n">
-        <v>255</v>
-      </c>
-      <c r="I24" s="13"/>
-    </row>
-    <row r="25" customFormat="false" ht="47.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A25" s="9"/>
-      <c r="B25" s="9"/>
-      <c r="C25" s="8" t="s">
+    <row r="25" customFormat="false" ht="32.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A25" s="14"/>
+      <c r="B25" s="14"/>
+      <c r="C25" s="17" t="s">
         <v>59</v>
       </c>
-      <c r="D25" s="8"/>
-      <c r="E25" s="8" t="s">
+      <c r="D25" s="17"/>
+      <c r="E25" s="17" t="s">
         <v>60</v>
       </c>
-      <c r="F25" s="8"/>
-      <c r="G25" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="H25" s="8"/>
-      <c r="I25" s="13"/>
-    </row>
-    <row r="26" customFormat="false" ht="38.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="F25" s="17"/>
+      <c r="G25" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="H25" s="17" t="n">
+        <v>255</v>
+      </c>
+      <c r="I25" s="18"/>
+    </row>
+    <row r="26" customFormat="false" ht="30.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="14" t="s">
         <v>61</v>
       </c>
@@ -1266,146 +1221,70 @@
         <v>11</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="40.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="27" customFormat="false" ht="31.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A27" s="14"/>
       <c r="B27" s="14"/>
-      <c r="C27" s="8" t="s">
+      <c r="C27" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="D27" s="8"/>
-      <c r="E27" s="8" t="s">
+      <c r="D27" s="6"/>
+      <c r="E27" s="6" t="s">
         <v>65</v>
       </c>
-      <c r="F27" s="8"/>
-      <c r="G27" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="H27" s="8" t="n">
-        <v>255</v>
-      </c>
-      <c r="I27" s="17"/>
-    </row>
-    <row r="28" customFormat="false" ht="40.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A28" s="14" t="s">
+      <c r="F27" s="6"/>
+      <c r="G27" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="H27" s="6" t="n">
+        <v>255</v>
+      </c>
+      <c r="I27" s="19"/>
+    </row>
+    <row r="28" customFormat="false" ht="30.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A28" s="14"/>
+      <c r="B28" s="14"/>
+      <c r="C28" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="B28" s="14"/>
-      <c r="C28" s="15" t="s">
+      <c r="D28" s="6"/>
+      <c r="E28" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="D28" s="15"/>
-      <c r="E28" s="15" t="s">
-        <v>68</v>
-      </c>
-      <c r="F28" s="15"/>
-      <c r="G28" s="15" t="s">
-        <v>10</v>
-      </c>
-      <c r="H28" s="15"/>
-      <c r="I28" s="16" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="29" customFormat="false" ht="32.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="F28" s="6"/>
+      <c r="G28" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="H28" s="6"/>
+      <c r="I28" s="19"/>
+    </row>
+    <row r="29" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A29" s="14"/>
       <c r="B29" s="14"/>
-      <c r="C29" s="18" t="s">
+      <c r="C29" s="17" t="s">
+        <v>68</v>
+      </c>
+      <c r="D29" s="17"/>
+      <c r="E29" s="17" t="s">
         <v>69</v>
       </c>
-      <c r="D29" s="18"/>
-      <c r="E29" s="18" t="s">
-        <v>70</v>
-      </c>
-      <c r="F29" s="18"/>
-      <c r="G29" s="18" t="s">
-        <v>14</v>
-      </c>
-      <c r="H29" s="18" t="n">
-        <v>255</v>
-      </c>
-      <c r="I29" s="19"/>
-    </row>
-    <row r="30" customFormat="false" ht="30.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A30" s="14" t="s">
-        <v>71</v>
-      </c>
-      <c r="B30" s="14"/>
-      <c r="C30" s="15" t="s">
-        <v>72</v>
-      </c>
-      <c r="D30" s="15"/>
-      <c r="E30" s="15" t="s">
-        <v>73</v>
-      </c>
-      <c r="F30" s="15"/>
-      <c r="G30" s="15" t="s">
-        <v>10</v>
-      </c>
-      <c r="H30" s="15"/>
-      <c r="I30" s="16" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="31" customFormat="false" ht="31.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A31" s="14"/>
-      <c r="B31" s="14"/>
-      <c r="C31" s="6" t="s">
-        <v>74</v>
-      </c>
-      <c r="D31" s="6"/>
-      <c r="E31" s="6" t="s">
-        <v>75</v>
-      </c>
-      <c r="F31" s="6"/>
-      <c r="G31" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="H31" s="6" t="n">
-        <v>255</v>
-      </c>
-      <c r="I31" s="20"/>
-    </row>
-    <row r="32" customFormat="false" ht="30.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A32" s="14"/>
-      <c r="B32" s="14"/>
-      <c r="C32" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="D32" s="6"/>
-      <c r="E32" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="F32" s="6"/>
-      <c r="G32" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="H32" s="6"/>
-      <c r="I32" s="20"/>
-    </row>
-    <row r="33" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A33" s="14"/>
-      <c r="B33" s="14"/>
-      <c r="C33" s="18" t="s">
-        <v>78</v>
-      </c>
-      <c r="D33" s="18"/>
-      <c r="E33" s="18" t="s">
-        <v>79</v>
-      </c>
-      <c r="F33" s="18"/>
-      <c r="G33" s="18" t="s">
-        <v>14</v>
-      </c>
-      <c r="H33" s="18" t="n">
-        <v>255</v>
-      </c>
-      <c r="I33" s="19"/>
-    </row>
-    <row r="34" customFormat="false" ht="30.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="35" customFormat="false" ht="30.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="36" customFormat="false" ht="33" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+      <c r="F29" s="17"/>
+      <c r="G29" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="H29" s="17" t="n">
+        <v>255</v>
+      </c>
+      <c r="I29" s="18"/>
+    </row>
+    <row r="30" customFormat="false" ht="30.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="31" customFormat="false" ht="30.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="32" customFormat="false" ht="33" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048573" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
-  <mergeCells count="75">
+  <mergeCells count="65">
     <mergeCell ref="A1:I2"/>
     <mergeCell ref="A3:B3"/>
     <mergeCell ref="C3:D3"/>
@@ -1426,17 +1305,16 @@
     <mergeCell ref="E9:F9"/>
     <mergeCell ref="C10:D10"/>
     <mergeCell ref="E10:F10"/>
-    <mergeCell ref="A11:B12"/>
+    <mergeCell ref="A11:B18"/>
     <mergeCell ref="C11:D11"/>
     <mergeCell ref="E11:F11"/>
     <mergeCell ref="C12:D12"/>
     <mergeCell ref="E12:F12"/>
-    <mergeCell ref="A13:B20"/>
+    <mergeCell ref="I12:I18"/>
     <mergeCell ref="C13:D13"/>
     <mergeCell ref="E13:F13"/>
     <mergeCell ref="C14:D14"/>
     <mergeCell ref="E14:F14"/>
-    <mergeCell ref="I14:I20"/>
     <mergeCell ref="C15:D15"/>
     <mergeCell ref="E15:F15"/>
     <mergeCell ref="C16:D16"/>
@@ -1445,42 +1323,33 @@
     <mergeCell ref="E17:F17"/>
     <mergeCell ref="C18:D18"/>
     <mergeCell ref="E18:F18"/>
+    <mergeCell ref="A19:B20"/>
     <mergeCell ref="C19:D19"/>
     <mergeCell ref="E19:F19"/>
     <mergeCell ref="C20:D20"/>
     <mergeCell ref="E20:F20"/>
-    <mergeCell ref="A21:B22"/>
+    <mergeCell ref="A21:B23"/>
     <mergeCell ref="C21:D21"/>
     <mergeCell ref="E21:F21"/>
     <mergeCell ref="C22:D22"/>
     <mergeCell ref="E22:F22"/>
-    <mergeCell ref="A23:B25"/>
+    <mergeCell ref="I22:I23"/>
     <mergeCell ref="C23:D23"/>
     <mergeCell ref="E23:F23"/>
+    <mergeCell ref="A24:B25"/>
     <mergeCell ref="C24:D24"/>
     <mergeCell ref="E24:F24"/>
-    <mergeCell ref="I24:I25"/>
     <mergeCell ref="C25:D25"/>
     <mergeCell ref="E25:F25"/>
-    <mergeCell ref="A26:B27"/>
+    <mergeCell ref="A26:B29"/>
     <mergeCell ref="C26:D26"/>
     <mergeCell ref="E26:F26"/>
     <mergeCell ref="C27:D27"/>
     <mergeCell ref="E27:F27"/>
-    <mergeCell ref="A28:B29"/>
     <mergeCell ref="C28:D28"/>
     <mergeCell ref="E28:F28"/>
     <mergeCell ref="C29:D29"/>
     <mergeCell ref="E29:F29"/>
-    <mergeCell ref="A30:B33"/>
-    <mergeCell ref="C30:D30"/>
-    <mergeCell ref="E30:F30"/>
-    <mergeCell ref="C31:D31"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="C32:D32"/>
-    <mergeCell ref="E32:F32"/>
-    <mergeCell ref="C33:D33"/>
-    <mergeCell ref="E33:F33"/>
   </mergeCells>
   <printOptions headings="false" gridLines="true" gridLinesSet="true" horizontalCentered="true" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>

<commit_message>
Maj dico de données : ajout de la classe répondre
</commit_message>
<xml_diff>
--- a/bdd/dico_de_donnees.xlsx
+++ b/bdd/dico_de_donnees.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="71">
   <si>
     <t xml:space="preserve">DICTIONNAIRE DE DONNEES</t>
   </si>
@@ -230,6 +230,9 @@
   </si>
   <si>
     <t xml:space="preserve">contenu du commentaire du sujet</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Répondre</t>
   </si>
 </sst>
 </file>
@@ -723,11 +726,11 @@
   </sheetPr>
   <dimension ref="A1:I1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A19" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H30" activeCellId="0" sqref="H30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.4609375" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.48046875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="28.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="28.98"/>
@@ -1276,15 +1279,36 @@
       </c>
       <c r="I29" s="18"/>
     </row>
-    <row r="30" customFormat="false" ht="30.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="31" customFormat="false" ht="30.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="32" customFormat="false" ht="33" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="30" customFormat="false" ht="30.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A30" s="14" t="s">
+        <v>70</v>
+      </c>
+      <c r="B30" s="14"/>
+      <c r="C30" s="15" t="s">
+        <v>50</v>
+      </c>
+      <c r="D30" s="15"/>
+      <c r="E30" s="15" t="s">
+        <v>63</v>
+      </c>
+      <c r="F30" s="15"/>
+      <c r="G30" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="H30" s="15"/>
+      <c r="I30" s="16" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="1048570" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048571" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048572" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048573" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
-  <mergeCells count="65">
+  <mergeCells count="68">
     <mergeCell ref="A1:I2"/>
     <mergeCell ref="A3:B3"/>
     <mergeCell ref="C3:D3"/>
@@ -1350,6 +1374,9 @@
     <mergeCell ref="E28:F28"/>
     <mergeCell ref="C29:D29"/>
     <mergeCell ref="E29:F29"/>
+    <mergeCell ref="A30:B30"/>
+    <mergeCell ref="C30:D30"/>
+    <mergeCell ref="E30:F30"/>
   </mergeCells>
   <printOptions headings="false" gridLines="true" gridLinesSet="true" horizontalCentered="true" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>